<commit_message>
calculo III gabarito VR e resultados finais
</commit_message>
<xml_diff>
--- a/calculoIII/2025-1/2025-1-calculoIII-A-notas.xlsx
+++ b/calculoIII/2025-1/2025-1-calculoIII-A-notas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t xml:space="preserve">Matrícula</t>
   </si>
@@ -82,25 +82,25 @@
     <t xml:space="preserve">amauri_junior@id.uff.br</t>
   </si>
   <si>
+    <t xml:space="preserve">ANNA KAROLINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NETO DOS SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annaneto@id.uff.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTHUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEIXOTO FIGUEIREDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arthurpf@id.uff.br</t>
+  </si>
+  <si>
     <t xml:space="preserve">ausente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANNA KAROLINA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NETO DOS SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annaneto@id.uff.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARTHUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEIXOTO FIGUEIREDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arthurpf@id.uff.br</t>
   </si>
   <si>
     <t xml:space="preserve">BRUNO</t>
@@ -679,7 +679,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -805,8 +805,8 @@
       <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
+      <c r="G3" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>3.8</v>
@@ -820,15 +820,15 @@
       </c>
       <c r="K3" s="2" t="n">
         <f aca="false">IF(SUM(F3:I3)/2&gt;10,10,SUM(F3:I3)/2)</f>
-        <v>5.15</v>
+        <v>8.65</v>
       </c>
       <c r="L3" s="3" t="str">
         <f aca="false">IF(K3&lt;4,"REP.",IF(K3&lt;6,"VS","APR."))</f>
-        <v>VS</v>
+        <v>APR.</v>
       </c>
       <c r="N3" s="2" t="n">
         <f aca="false">IF(OR(K3&gt;=6,K3&lt;4),K3,IF(M3&gt;=6,6,(K3+M3)/2))</f>
-        <v>2.575</v>
+        <v>8.65</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -842,13 +842,13 @@
         <v>17160671708</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
@@ -890,13 +890,13 @@
         <v>12867997755</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>2.1</v>
@@ -905,7 +905,7 @@
         <v>2.5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J5" s="1" t="str">
         <f aca="false">IF(I5="ausente",I5,IF(H5="ausente",ROUND(I5*10/7,1),IF(I5+H5&gt;10,10,I5+H5)))</f>
@@ -950,7 +950,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>5</v>
@@ -1328,7 +1328,7 @@
         <v>53</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>2.7</v>
+        <v>8</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>2.5</v>
@@ -1342,15 +1342,15 @@
       </c>
       <c r="K14" s="2" t="n">
         <f aca="false">IF(SUM(F14:I14)/2&gt;10,10,SUM(F14:I14)/2)</f>
-        <v>5.35</v>
+        <v>8</v>
       </c>
       <c r="L14" s="3" t="str">
         <f aca="false">IF(K14&lt;4,"REP.",IF(K14&lt;6,"VS","APR."))</f>
-        <v>VS</v>
+        <v>APR.</v>
       </c>
       <c r="N14" s="2" t="n">
         <f aca="false">IF(OR(K14&gt;=6,K14&lt;4),K14,IF(M14&gt;=6,6,(K14+M14)/2))</f>
-        <v>2.675</v>
+        <v>8</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -1373,13 +1373,13 @@
         <v>56</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J15" s="1" t="str">
         <f aca="false">IF(I15="ausente",I15,IF(H15="ausente",ROUND(I15*10/7,1),IF(I15+H15&gt;10,10,I15+H15)))</f>
@@ -1510,8 +1510,8 @@
       <c r="E18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>20</v>
+      <c r="G18" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>3.5</v>
@@ -1525,15 +1525,15 @@
       </c>
       <c r="K18" s="2" t="n">
         <f aca="false">IF(SUM(F18:I18)/2&gt;10,10,SUM(F18:I18)/2)</f>
-        <v>4.1</v>
+        <v>7.1</v>
       </c>
       <c r="L18" s="3" t="str">
         <f aca="false">IF(K18&lt;4,"REP.",IF(K18&lt;6,"VS","APR."))</f>
-        <v>VS</v>
+        <v>APR.</v>
       </c>
       <c r="N18" s="2" t="n">
         <f aca="false">IF(OR(K18&gt;=6,K18&lt;4),K18,IF(M18&gt;=6,6,(K18+M18)/2))</f>
-        <v>2.05</v>
+        <v>7.1</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -1558,8 +1558,8 @@
       <c r="F19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>20</v>
+      <c r="G19" s="1" t="n">
+        <v>4.6</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>2.3</v>
@@ -1573,15 +1573,15 @@
       </c>
       <c r="K19" s="2" t="n">
         <f aca="false">IF(SUM(F19:I19)/2&gt;10,10,SUM(F19:I19)/2)</f>
-        <v>5.15</v>
+        <v>7.45</v>
       </c>
       <c r="L19" s="3" t="str">
         <f aca="false">IF(K19&lt;4,"REP.",IF(K19&lt;6,"VS","APR."))</f>
-        <v>VS</v>
+        <v>APR.</v>
       </c>
       <c r="N19" s="2" t="n">
         <f aca="false">IF(OR(K19&gt;=6,K19&lt;4),K19,IF(M19&gt;=6,6,(K19+M19)/2))</f>
-        <v>2.575</v>
+        <v>7.45</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -1748,13 +1748,13 @@
         <v>80</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J23" s="1" t="str">
         <f aca="false">IF(I23="ausente",I23,IF(H23="ausente",ROUND(I23*10/7,1),IF(I23+H23&gt;10,10,I23+H23)))</f>
@@ -2030,7 +2030,7 @@
         <v>98</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>2.1</v>
+        <v>7</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>2.8</v>
@@ -2044,15 +2044,15 @@
       </c>
       <c r="K29" s="2" t="n">
         <f aca="false">IF(SUM(F29:I29)/2&gt;10,10,SUM(F29:I29)/2)</f>
-        <v>5.2</v>
+        <v>7.65</v>
       </c>
       <c r="L29" s="3" t="str">
         <f aca="false">IF(K29&lt;4,"REP.",IF(K29&lt;6,"VS","APR."))</f>
-        <v>VS</v>
+        <v>APR.</v>
       </c>
       <c r="N29" s="2" t="n">
         <f aca="false">IF(OR(K29&gt;=6,K29&lt;4),K29,IF(M29&gt;=6,6,(K29+M29)/2))</f>
-        <v>2.6</v>
+        <v>7.65</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
@@ -2074,8 +2074,8 @@
       <c r="E30" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>20</v>
+      <c r="G30" s="1" t="n">
+        <v>4.6</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>3.8</v>
@@ -2089,15 +2089,15 @@
       </c>
       <c r="K30" s="2" t="n">
         <f aca="false">IF(SUM(F30:I30)/2&gt;10,10,SUM(F30:I30)/2)</f>
-        <v>4.9</v>
+        <v>7.2</v>
       </c>
       <c r="L30" s="3" t="str">
         <f aca="false">IF(K30&lt;4,"REP.",IF(K30&lt;6,"VS","APR."))</f>
-        <v>VS</v>
+        <v>APR.</v>
       </c>
       <c r="N30" s="2" t="n">
         <f aca="false">IF(OR(K30&gt;=6,K30&lt;4),K30,IF(M30&gt;=6,6,(K30+M30)/2))</f>
-        <v>2.45</v>
+        <v>7.2</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
@@ -2176,16 +2176,16 @@
       <c r="H32" s="1" t="n">
         <v>3.8</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="1" t="str">
+      <c r="I32" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J32" s="1" t="n">
         <f aca="false">IF(I32="ausente",I32,IF(H32="ausente",ROUND(I32*10/7,1),IF(I32+H32&gt;10,10,I32+H32)))</f>
-        <v>ausente</v>
+        <v>9.8</v>
       </c>
       <c r="K32" s="2" t="n">
         <f aca="false">IF(SUM(F32:I32)/2&gt;10,10,SUM(F32:I32)/2)</f>
-        <v>6.85</v>
+        <v>9.85</v>
       </c>
       <c r="L32" s="3" t="str">
         <f aca="false">IF(K32&lt;4,"REP.",IF(K32&lt;6,"VS","APR."))</f>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="N32" s="2" t="n">
         <f aca="false">IF(OR(K32&gt;=6,K32&lt;4),K32,IF(M32&gt;=6,6,(K32+M32)/2))</f>
-        <v>6.85</v>
+        <v>9.85</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>

</xml_diff>